<commit_message>
Bug Fixed in SubSuite drag/drop issue
</commit_message>
<xml_diff>
--- a/src/main/resources/project/Suite 1.xlsx
+++ b/src/main/resources/project/Suite 1.xlsx
@@ -12,7 +12,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
+  <si>
+    <t>Sub-Suite: Sub-Suite 1</t>
+  </si>
   <si>
     <t>Scenario: Test Suite</t>
   </si>
@@ -44,38 +47,91 @@
     <t>checkFileContainsKeyword</t>
   </si>
   <si>
-    <t>sad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   if (new KeyCodeCombination(KeyCode.S, KeyCombination.CONTROL_DOWN).match(event)) {
-                            TreeItem&lt;TestNode&gt; selected = treeView.getSelectionModel().getSelectedItem();
-                            if (selected != null &amp;&amp; selected.getValue().getType() == NodeType.TEST_SCENARIO) {
-                                saveTestScenario(selected);
-                            }
-                            saveProject(); // export included
-                            event.consume();
-                        }
-                    });
-                }
-            });
-        });
-        tableView.getColumns().setAll(itemColumn, objectColumn, actionColumn, descriptionColumn, inputColumn);
-        tableView.setFixedCellSize(25);
-    }
-    @FXML
-    private void handleNewSuite(ActionEvent event) {
-        TreeItem&lt;TestNode&gt; root = treeView.getRoot();
-        if (root != null) {
-            int suiteCount = root.getChildren().size() + 1;
-            TreeItem&lt;TestNode&gt; newSuite = new TreeItem&lt;&gt;(new TestNode("Suite " + suiteCount, NodeType.SUITE));
-            newSuite.setExpanded(true);
-            root.getChildren().add(newSuite);
+    <t>2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell.setOnDragDropped(event -&gt; {
+    Dragboard db = event.getDragboard();
+    boolean success = false;
+    if (db.hasString()) {
+        TreeItem&lt;TestNode&gt; draggedItem = findItem(treeView.getRoot(), db.getString());
+        TreeItem&lt;TestNode&gt; targetItem = cell.getTreeItem();
+        if (draggedItem != null &amp;&amp; targetItem != null &amp;&amp; isValidDrop(draggedItem, targetItem)) {
+            // Capture old key BEFORE moving
+            String oldKey = makeKey(draggedItem);
+            // Move the node once
+            draggedItem.getParent().getChildren().remove(draggedItem);
+            targetItem.getChildren().add(draggedItem);
+            // Compute new key AFTER move
+            String newKey = makeKey(draggedItem);
+            // Move scenario data to new key
+            if (scenarioSteps.containsKey(oldKey)) {
+                scenarioSteps.put(newKey, scenarioSteps.remove(oldKey));
+            }
+            if (scenarioColumns.containsKey(oldKey)) {
+                scenarioColumns.put(newKey, scenarioColumns.remove(oldKey));
+            }
+            success = true;
+        } else {
+            showError("Invalid drop target for " +
+                    (draggedItem != null ? draggedItem.getValue().getName() : ""));
         }
     }
+    event.setDropCompleted(success);
+    event.consume();
+});
 </t>
   </si>
   <si>
-    <t>sd</t>
+    <t>Scenario: TestSuite</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell.setOnDragDropped(event -&gt; {
+    Dragboard db = event.getDragboard();
+    boolean success = false;
+    if (db.hasString()) {
+        TreeItem&lt;TestNode&gt; draggedItem = findItem(treeView.getRoot(), db.getString());
+        TreeItem&lt;TestNode&gt; targetItem = cell.getTreeItem();
+        if (draggedItem != null &amp;&amp; targetItem != null &amp;&amp; isValidDrop(draggedItem, targetItem)) {
+            // Capture old key BEFORE moving
+            String oldKey = makeKey(draggedItem);
+            // Move the node once
+            draggedItem.getParent().getChildren().remove(draggedItem);
+            targetItem.getChildren().add(draggedItem);
+            // Compute new key AFTER move
+            String newKey = makeKey(draggedItem);
+            // Move scenario data to new key
+            if (scenarioSteps.containsKey(oldKey)) {
+                scenarioSteps.put(newKey, scenarioSteps.remove(oldKey));
+            }
+            if (scenarioColumns.containsKey(oldKey)) {
+                scenarioColumns.put(newKey, scenarioColumns.remove(oldKey));
+            }
+            success = true;
+        } else {
+            showError("Invalid drop target for " +
+                    (draggedItem != null ? draggedItem.getValue().getName() : ""));
+        }
+    }
+    event.setDropCompleted(success);
+    event.consume();
+});
+</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>executeQuery</t>
   </si>
 </sst>
 </file>
@@ -120,7 +176,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -135,40 +191,150 @@
       <c r="A2" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>6</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="B3" t="s" s="0">
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="B4" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="C4" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="E3" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s" s="0">
+      <c r="D4" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s" s="0">
         <v>12</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added fix in No Content issue for TestSuite and popup error for subsuite.
</commit_message>
<xml_diff>
--- a/src/main/resources/project/Suite 1.xlsx
+++ b/src/main/resources/project/Suite 1.xlsx
@@ -12,35 +12,41 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="15">
+  <si>
+    <t>Scenario: haha2</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>WebServer</t>
+  </si>
+  <si>
+    <t>sendRequest</t>
+  </si>
+  <si>
+    <t/>
+  </si>
   <si>
     <t>Scenario: Test Suite</t>
   </si>
   <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Object</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Input</t>
-  </si>
-  <si>
-    <t>gagaha</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -50,34 +56,7 @@
     <t>checkFileContainsKeyword</t>
   </si>
   <si>
-    <t xml:space="preserve">@FXML
-private void handleAddColumn(ActionEvent event) {
-    TreeItem&lt;TestNode&gt; selected = treeView.getSelectionModel().getSelectedItem();
-    if (selected == null || selected.getValue().getType() != NodeType.TEST_SCENARIO) {
-        showError("Extra columns can only be added inside a TestScenario.");
-        return;
-    }
-    String key = makeKey(selected);
-    String colName = "Extra" + (tableView.getColumns().size() - 4);
-    TableColumn&lt;TestStep, String&gt; extraColumn = new TableColumn&lt;&gt;(colName);
-    extraColumn.setCellValueFactory(cellData -&gt; cellData.getValue().getExtraProperty(colName));
-    extraColumn.setCellFactory(col -&gt; new AutoCommitTextFieldTableCell&lt;&gt;());
-    extraColumn.setOnEditCommit(evt -&gt; evt.getRowValue().setExtra(colName, evt.getNewValue()));
-    // ✅ Add context menu for renaming
-    MenuItem renameCol = new MenuItem("Rename…");
-    renameCol.setOnAction(e -&gt; {
-        TreeItem&lt;TestNode&gt; scenario = treeView.getSelectionModel().getSelectedItem();
-        handleRenameColumn(extraColumn, scenario);
-    });
-    extraColumn.setContextMenu(new ContextMenu(renameCol));
-    tableView.getColumns().add(extraColumn);
-    // Record column name for this scenario
-    scenarioColumns.computeIfAbsent(key, k -&gt; new ArrayList&lt;&gt;()).add(colName);
-}
-</t>
-  </si>
-  <si>
-    <t>asda</t>
+    <t>Sub-Suite: Sub-Suite 3</t>
   </si>
 </sst>
 </file>
@@ -122,7 +101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -149,48 +128,122 @@
       <c r="E2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="F2" t="s" s="0">
-        <v>6</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s" s="0">
         <v>7</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>8</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="C4" t="s" s="0">
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D4" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s" s="0">
+      <c r="B7" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="C7" t="s" s="0">
         <v>13</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix layout design + functionality of tableview arrange up/down
</commit_message>
<xml_diff>
--- a/src/main/resources/project/Suite 1.xlsx
+++ b/src/main/resources/project/Suite 1.xlsx
@@ -12,9 +12,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
-  <si>
-    <t>Scenario: LoginScreen</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+  <si>
+    <t>Scenario: Test Suite</t>
   </si>
   <si>
     <t>Item</t>
@@ -32,7 +32,7 @@
     <t>Input</t>
   </si>
   <si>
-    <t>Extra1</t>
+    <t>gag32</t>
   </si>
   <si>
     <t>1</t>
@@ -44,37 +44,69 @@
     <t>checkFileContainsKeyword</t>
   </si>
   <si>
-    <t>SUITE::Suite 1SUITE::Suite 1SUITE::Suite 1</t>
-  </si>
-  <si>
-    <t>gaga</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">// 👉 Enable drag-and-drop row reordering
+tableView.setRowFactory(tv -&gt; {
+    TableRow&lt;TestStep&gt; row = new TableRow&lt;&gt;();
+    row.setOnDragDetected(event -&gt; {
+        if (!row.isEmpty()) {
+            Dragboard db = row.startDragAndDrop(TransferMode.MOVE);
+            ClipboardContent cc = new ClipboardContent();
+            cc.putString(Integer.toString(row.getIndex()));
+            db.setContent(cc);
+            event.consume();
+        }
+    });
+    row.setOnDragOver(event -&gt; {
+        Dragboard db = event.getDragboard();
+        if (db.hasString()) {
+            int draggedIndex = Integer.parseInt(db.getString());
+            if (row.getIndex() != draggedIndex) {
+                event.acceptTransferModes(TransferMode.MOVE);
+                row.setStyle("-fx-background-color: lightgreen;");
+            }
+        }
+        event.consume();
+    });
+    row.setOnDragExited(event -&gt; row.setStyle(""));
+    row.setOnDragDropped(event -&gt; {
+        Dragboard db = event.getDragboard();
+        if (db.hasString()) {
+            int draggedIndex = Integer.parseInt(db.getString());
+            TestStep draggedStep = tableView.getItems().remove(draggedIndex);
+            int dropIndex = row.isEmpty() ? tableView.getItems().size() : row.getIndex();
+            tableView.getItems().add(dropIndex, draggedStep);
+            tableView.getSelectionModel().select(dropIndex);
+            event.setDropCompleted(true);
+        }
+        event.consume();
+    });
+    return row;
+});
+</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
+    <t>WebServer</t>
+  </si>
+  <si>
+    <t>sendRequest</t>
+  </si>
+  <si>
     <t>Database</t>
   </si>
   <si>
     <t>executeQuery</t>
   </si>
   <si>
-    <t>SUITE::Suite 1</t>
-  </si>
-  <si>
-    <t>haha</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>WebServer</t>
-  </si>
-  <si>
-    <t>sendRequest</t>
-  </si>
-  <si>
-    <t/>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -161,53 +193,53 @@
         <v>9</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="D5" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="C5" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>17</v>
-      </c>
       <c r="E5" t="s" s="0">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added drag and drop variablt to datasheet with working value inside.
</commit_message>
<xml_diff>
--- a/src/main/resources/project/Suite 1.xlsx
+++ b/src/main/resources/project/Suite 1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Scenario: Test Suite</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>gaga</t>
   </si>
 </sst>
 </file>
@@ -122,7 +125,7 @@
         <v>7</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stable TextField but Object running is failing
</commit_message>
<xml_diff>
--- a/src/main/resources/project/Suite 1.xlsx
+++ b/src/main/resources/project/Suite 1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Scenario: Test Suite</t>
   </si>
@@ -35,10 +35,13 @@
     <t>1</t>
   </si>
   <si>
-    <t/>
+    <t>FileSystem</t>
   </si>
   <si>
-    <t>gaga</t>
+    <t>checkFileContainsKeyword</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -119,13 +122,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added driven framework functionality with uuid features, loggers and everything, this is the most compact version.
</commit_message>
<xml_diff>
--- a/src/main/resources/project/Suite 1.xlsx
+++ b/src/main/resources/project/Suite 1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="9">
   <si>
     <t>Scenario: Test Suite</t>
   </si>
@@ -32,16 +32,13 @@
     <t>Input</t>
   </si>
   <si>
-    <t>1</t>
+    <t/>
   </si>
   <si>
     <t>FileSystem</t>
   </si>
   <si>
     <t>checkFileContainsKeyword</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
@@ -86,7 +83,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -119,16 +116,67 @@
         <v>6</v>
       </c>
       <c r="B3" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C4" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="D3" t="s" s="0">
-        <v>9</v>
+      <c r="D4" t="s" s="0">
+        <v>6</v>
       </c>
-      <c r="E3" t="s" s="0">
-        <v>9</v>
+      <c r="E4" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>